<commit_message>
Atualizando os valores da lista de produtos
</commit_message>
<xml_diff>
--- a/commodities_atualizada.xlsx
+++ b/commodities_atualizada.xlsx
@@ -465,7 +465,7 @@
         <v>85.31999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>53.54</v>
+        <v>53.88</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -481,7 +481,7 @@
         <v>163.59</v>
       </c>
       <c r="C3" t="n">
-        <v>146.71</v>
+        <v>146.99</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -497,7 +497,7 @@
         <v>282.2</v>
       </c>
       <c r="C4" t="n">
-        <v>199.8</v>
+        <v>199.65</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -513,7 +513,7 @@
         <v>424.37</v>
       </c>
       <c r="C5" t="n">
-        <v>438.53</v>
+        <v>439.3</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -529,7 +529,7 @@
         <v>497.76</v>
       </c>
       <c r="C6" t="n">
-        <v>404.75</v>
+        <v>408.42</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>136.23</v>
       </c>
       <c r="C7" t="n">
-        <v>145.19</v>
+        <v>149.24</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -561,7 +561,7 @@
         <v>1092.87</v>
       </c>
       <c r="C8" t="n">
-        <v>816.58</v>
+        <v>818.1799999999999</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -577,7 +577,7 @@
         <v>321.77</v>
       </c>
       <c r="C9" t="n">
-        <v>312.45</v>
+        <v>311.63</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>

</xml_diff>